<commit_message>
att hotel csv 12/4
</commit_message>
<xml_diff>
--- a/data/hotel.xlsx
+++ b/data/hotel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar\OneDrive\Desktop\Salva\EGI FEUP\1ºano 2º semestre\Programação de Computadores II\Trabalho de grupo\PCII_grupo_T1G5\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62BDE7FF-8113-4553-AF8E-F4ED1C0D942C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D567F-4A77-41C1-BA87-B51E255AF795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11736" yWindow="36" windowWidth="11304" windowHeight="8880" xr2:uid="{129760C3-D296-4E01-8ABC-B4EAB38CBA59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>code</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Aveiro</t>
+  </si>
+  <si>
+    <t>H4</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A327F7-394E-447A-A6F7-CAEF4BAB0726}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +501,7 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>968693641</v>
+        <v>968693643</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -519,6 +522,23 @@
       </c>
       <c r="E4">
         <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>638</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>968693641</v>
+      </c>
+      <c r="E5">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>